<commit_message>
test app.R and partially solved insertUI
</commit_message>
<xml_diff>
--- a/WorkingPath.xlsx
+++ b/WorkingPath.xlsx
@@ -4,26 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>Place</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>PJSOC Bashneft</t>
   </si>
@@ -31,7 +24,103 @@
     <t>SPB Ltd.</t>
   </si>
   <si>
-    <t>GC Aspec</t>
+    <t>company</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>DLP System</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>Zecurion</t>
+  </si>
+  <si>
+    <t>Video conferencing system</t>
+  </si>
+  <si>
+    <t>Polycom &amp; Microsoft</t>
+  </si>
+  <si>
+    <t>Document automation system</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Consolidations Active Directory services</t>
+  </si>
+  <si>
+    <t>VMware</t>
+  </si>
+  <si>
+    <t>ITIL</t>
+  </si>
+  <si>
+    <t>ITSM</t>
+  </si>
+  <si>
+    <t>Polycom</t>
+  </si>
+  <si>
+    <t>Microsoft servers &amp; services</t>
+  </si>
+  <si>
+    <t>Information security</t>
+  </si>
+  <si>
+    <t>Project management</t>
+  </si>
+  <si>
+    <t>Aspec Group Company</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>IT infrastructure</t>
+  </si>
+  <si>
+    <t>CRM system</t>
+  </si>
+  <si>
+    <t>Video surveillance</t>
+  </si>
+  <si>
+    <t>Access control systems</t>
+  </si>
+  <si>
+    <t>keySkills</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Freelance</t>
+  </si>
+  <si>
+    <t>BOSS-Referent</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>experience</t>
   </si>
 </sst>
 </file>
@@ -39,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-419]mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-419]mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -72,7 +161,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -377,144 +466,402 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1">
+        <v>39417</v>
+      </c>
+      <c r="C2" s="1">
+        <v>39660</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>39417</v>
-      </c>
-      <c r="B2" s="1">
-        <v>39660</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" s="1">
+        <v>39661</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40524</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40544</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>39661</v>
-      </c>
-      <c r="B3" s="1">
-        <v>40524</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>40544</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="B5" s="1">
+        <v>43101</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>